<commit_message>
修改BUG: 02_led_drv_for_boards\board_am335x.c; 添加2视频: 15.1_AM335X按键驱动程序(查询方式).mp4, 15.2_RK3288按键驱动程序(查询方式).mp4
</commit_message>
<xml_diff>
--- a/04_快速入门(正式开始)/02_嵌入式Linux驱动开发基础知识/doc_pic/pic/05.具体单板的GPIO操作方法/RK3288_RK3399_GPIO寄存器列表.xlsx
+++ b/04_快速入门(正式开始)/02_嵌入式Linux驱动开发基础知识/doc_pic/pic/05.具体单板的GPIO操作方法/RK3288_RK3399_GPIO寄存器列表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\资料\设计方案\视频教程\2019全系视频\裸机视频\02.第1个ARM裸板程序及引申\doc_pic\第03节_具体单板的GPIO操作方法\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\01_all_series_quickstart\04_快速入门(正式开始)\02_嵌入式Linux驱动开发基础知识\doc_pic\pic\05.具体单板的GPIO操作方法\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E138A7-D59A-4E68-B530-E8DFC3623AE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACADC4E-FA3D-4F99-8D49-A29E3D261BC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F924F868-21D7-42CC-A3BB-1A2FF72BFB5D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="185">
   <si>
     <t>Module</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0xFF7E0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0xFF7F0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,357 +281,370 @@
     <t xml:space="preserve">GRF_GPIO7A_IOMUX </t>
   </si>
   <si>
+    <t>GRF_GPIO7CL_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO7CH_IOMUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRF_GPIO8B_IOMUX </t>
+  </si>
+  <si>
+    <t>0x000c</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>0x0014</t>
+  </si>
+  <si>
+    <t>0x0018</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>0x0024</t>
+  </si>
+  <si>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x002c</t>
+  </si>
+  <si>
+    <t>0x0030</t>
+  </si>
+  <si>
+    <t>0x0034</t>
+  </si>
+  <si>
+    <t>0x0038</t>
+  </si>
+  <si>
+    <t>0x003c</t>
+  </si>
+  <si>
+    <t>0x0044</t>
+  </si>
+  <si>
+    <t>0x0048</t>
+  </si>
+  <si>
+    <t>0x0050</t>
+  </si>
+  <si>
+    <t>0x0054</t>
+  </si>
+  <si>
+    <t>0x005c</t>
+  </si>
+  <si>
+    <t>0x0060</t>
+  </si>
+  <si>
+    <t>0x0064</t>
+  </si>
+  <si>
+    <t>0x006c</t>
+  </si>
+  <si>
+    <t>0x0070</t>
+  </si>
+  <si>
+    <t>0x0074</t>
+  </si>
+  <si>
+    <t>0x0078</t>
+  </si>
+  <si>
+    <t>GPIO1D iomux control</t>
+  </si>
+  <si>
+    <t>GPIO2A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO2B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO2C iomux control</t>
+  </si>
+  <si>
+    <t>GPIO3A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO3B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO3C iomux control</t>
+  </si>
+  <si>
+    <t>GPIO3D iomux control</t>
+  </si>
+  <si>
+    <t>GPIO4A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO4B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO4C iomux control</t>
+  </si>
+  <si>
+    <t>GPIO4D iomux control</t>
+  </si>
+  <si>
+    <t>GPIO5B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO5C iomux control</t>
+  </si>
+  <si>
+    <t>GPIO6A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO6B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO6C iomux control</t>
+  </si>
+  <si>
+    <t>GPIO7A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO7B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO7CL iomux control</t>
+  </si>
+  <si>
+    <t>GPIO7CH iomux control</t>
+  </si>
+  <si>
+    <t>GPIO8A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO8B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO_SWPORTA_DR</t>
+  </si>
+  <si>
+    <t>GPIO_SWPORTA_DDR</t>
+  </si>
+  <si>
+    <t>GPIO_EXT_PORTA</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>Port A data register</t>
+  </si>
+  <si>
+    <t>Port A data direction register</t>
+  </si>
+  <si>
+    <t>Port A clear interrupt register</t>
+  </si>
+  <si>
+    <t>RK3288</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RK3399</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF310000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF720000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF788000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMUGRF_GPIO0A_IOMUX</t>
+  </si>
+  <si>
+    <t>PMUGRF_GPIO0B_IOMUX</t>
+  </si>
+  <si>
+    <t>PMUGRF_GPIO1A_IOMUX</t>
+  </si>
+  <si>
+    <t>PMUGRF_GPIO1B_IOMUX</t>
+  </si>
+  <si>
+    <t>PMUGRF_GPIO1C_IOMUX</t>
+  </si>
+  <si>
+    <t>0x00000</t>
+  </si>
+  <si>
+    <t>0x00004</t>
+  </si>
+  <si>
+    <t>0x00010</t>
+  </si>
+  <si>
+    <t>0x00014</t>
+  </si>
+  <si>
+    <t>0x00018</t>
+  </si>
+  <si>
+    <t>GPIO0A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO0B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO1A iomux control</t>
+  </si>
+  <si>
+    <t>GPIO1B iomux control</t>
+  </si>
+  <si>
+    <t>GPIO1C iomux control</t>
+  </si>
+  <si>
+    <t>0x0104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRU_CLKGATE_CON31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x037c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GRF_GPIO2A_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO2B_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO2C_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO2D_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO3A_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO3B_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO3C_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO3D_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO4A_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO4B_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO4C_IOMUX</t>
+  </si>
+  <si>
+    <t>GRF_GPIO4D_IOMUX</t>
+  </si>
+  <si>
+    <t>0x0e000</t>
+  </si>
+  <si>
+    <t>0x0e004</t>
+  </si>
+  <si>
+    <t>0x0e008</t>
+  </si>
+  <si>
+    <t>0x0e00c</t>
+  </si>
+  <si>
+    <t>0x0e010</t>
+  </si>
+  <si>
+    <t>0x0e014</t>
+  </si>
+  <si>
+    <t>0x0e018</t>
+  </si>
+  <si>
+    <t>0x0e01c</t>
+  </si>
+  <si>
+    <t>0x0e020</t>
+  </si>
+  <si>
+    <t>0x0e024</t>
+  </si>
+  <si>
+    <t>0x0e028</t>
+  </si>
+  <si>
+    <t>0x0e02c</t>
+  </si>
+  <si>
+    <t>GPIO2D iomux control</t>
+  </si>
+  <si>
+    <t>使能GPIO0～1的时钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使能GPIO2～4的时钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMUCRU_CLKGATE_CON1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">GRF_GPIO8A_IOMUX </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0080</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO_SWPORTA_DDR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">GRF_GPIO7B_IOMUX </t>
-  </si>
-  <si>
-    <t>GRF_GPIO7CL_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO7CH_IOMUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRF_GPIO8B_IOMUX </t>
-  </si>
-  <si>
-    <t>0x000c</t>
-  </si>
-  <si>
-    <t>0x0010</t>
-  </si>
-  <si>
-    <t>0x0014</t>
-  </si>
-  <si>
-    <t>0x0018</t>
-  </si>
-  <si>
-    <t>0x0020</t>
-  </si>
-  <si>
-    <t>0x0024</t>
-  </si>
-  <si>
-    <t>0x0028</t>
-  </si>
-  <si>
-    <t>0x002c</t>
-  </si>
-  <si>
-    <t>0x0030</t>
-  </si>
-  <si>
-    <t>0x0034</t>
-  </si>
-  <si>
-    <t>0x0038</t>
-  </si>
-  <si>
-    <t>0x003c</t>
-  </si>
-  <si>
-    <t>0x0044</t>
-  </si>
-  <si>
-    <t>0x0048</t>
-  </si>
-  <si>
-    <t>0x0050</t>
-  </si>
-  <si>
-    <t>0x0054</t>
-  </si>
-  <si>
-    <t>0x005c</t>
-  </si>
-  <si>
-    <t>0x0060</t>
-  </si>
-  <si>
-    <t>0x0064</t>
-  </si>
-  <si>
-    <t>0x006c</t>
-  </si>
-  <si>
-    <t>0x0070</t>
-  </si>
-  <si>
-    <t>0x0074</t>
-  </si>
-  <si>
-    <t>0x0078</t>
-  </si>
-  <si>
-    <t>GPIO1D iomux control</t>
-  </si>
-  <si>
-    <t>GPIO2A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO2B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO2C iomux control</t>
-  </si>
-  <si>
-    <t>GPIO3A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO3B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO3C iomux control</t>
-  </si>
-  <si>
-    <t>GPIO3D iomux control</t>
-  </si>
-  <si>
-    <t>GPIO4A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO4B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO4C iomux control</t>
-  </si>
-  <si>
-    <t>GPIO4D iomux control</t>
-  </si>
-  <si>
-    <t>GPIO5B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO5C iomux control</t>
-  </si>
-  <si>
-    <t>GPIO6A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO6B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO6C iomux control</t>
-  </si>
-  <si>
-    <t>GPIO7A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO7B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO7CL iomux control</t>
-  </si>
-  <si>
-    <t>GPIO7CH iomux control</t>
-  </si>
-  <si>
-    <t>GPIO8A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO8B iomux control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GPIO_SWPORTA_DR</t>
-  </si>
-  <si>
-    <t>GPIO_SWPORTA_DDR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GPIO_EXT_PORTA</t>
-  </si>
-  <si>
-    <t>0x0000</t>
-  </si>
-  <si>
-    <t>0x0004</t>
-  </si>
-  <si>
-    <t>Port A data register</t>
-  </si>
-  <si>
-    <t>Port A data direction register</t>
-  </si>
-  <si>
-    <t>Port A clear interrupt register</t>
-  </si>
-  <si>
-    <t>RK3288</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RK3399</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xFF310000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xFF720000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0xFF788000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMUGRF_GPIO0A_IOMUX</t>
-  </si>
-  <si>
-    <t>PMUGRF_GPIO0B_IOMUX</t>
-  </si>
-  <si>
-    <t>PMUGRF_GPIO1A_IOMUX</t>
-  </si>
-  <si>
-    <t>PMUGRF_GPIO1B_IOMUX</t>
-  </si>
-  <si>
-    <t>PMUGRF_GPIO1C_IOMUX</t>
-  </si>
-  <si>
-    <t>0x00000</t>
-  </si>
-  <si>
-    <t>0x00004</t>
-  </si>
-  <si>
-    <t>0x00010</t>
-  </si>
-  <si>
-    <t>0x00014</t>
-  </si>
-  <si>
-    <t>0x00018</t>
-  </si>
-  <si>
-    <t>GPIO0A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO0B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO1A iomux control</t>
-  </si>
-  <si>
-    <t>GPIO1B iomux control</t>
-  </si>
-  <si>
-    <t>GPIO1C iomux control</t>
-  </si>
-  <si>
-    <t>0x0104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CRU_CLKGATE_CON31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x037c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GRF_GPIO2A_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO2B_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO2C_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO2D_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO3A_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO3B_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO3C_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO3D_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO4A_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO4B_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO4C_IOMUX</t>
-  </si>
-  <si>
-    <t>GRF_GPIO4D_IOMUX</t>
-  </si>
-  <si>
-    <t>0x0e000</t>
-  </si>
-  <si>
-    <t>0x0e004</t>
-  </si>
-  <si>
-    <t>0x0e008</t>
-  </si>
-  <si>
-    <t>0x0e00c</t>
-  </si>
-  <si>
-    <t>0x0e010</t>
-  </si>
-  <si>
-    <t>0x0e014</t>
-  </si>
-  <si>
-    <t>0x0e018</t>
-  </si>
-  <si>
-    <t>0x0e01c</t>
-  </si>
-  <si>
-    <t>0x0e020</t>
-  </si>
-  <si>
-    <t>0x0e024</t>
-  </si>
-  <si>
-    <t>0x0e028</t>
-  </si>
-  <si>
-    <t>0x0e02c</t>
-  </si>
-  <si>
-    <t>GPIO2D iomux control</t>
-  </si>
-  <si>
-    <t>使能GPIO0～1的时钟</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使能GPIO2～4的时钟</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMUCRU_CLKGATE_CON1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">GRF_GPIO8A_IOMUX </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0080</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPIO_SWPORTA_DDR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF7E0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1121,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA688D0-13E2-4FD3-93DD-BD974EE4FB02}">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1183,24 +1192,24 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1213,35 +1222,35 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1254,200 +1263,200 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1458,13 +1467,13 @@
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1475,69 +1484,69 @@
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K37" s="2"/>
     </row>
@@ -1609,7 +1618,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
@@ -1620,7 +1629,7 @@
         <v>28</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
@@ -1628,13 +1637,13 @@
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="D49" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" t="s">
         <v>123</v>
-      </c>
-      <c r="E49" t="s">
-        <v>125</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
@@ -1642,13 +1651,13 @@
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D50" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
@@ -1656,13 +1665,13 @@
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
@@ -1675,7 +1684,7 @@
     </row>
     <row r="54" spans="3:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C54" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="3:13" x14ac:dyDescent="0.2">
@@ -1726,24 +1735,24 @@
     </row>
     <row r="60" spans="3:13" x14ac:dyDescent="0.2">
       <c r="J60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K60" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="3:13" x14ac:dyDescent="0.2">
       <c r="J61" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L61" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="3:13" x14ac:dyDescent="0.2">
@@ -1751,62 +1760,62 @@
         <v>17</v>
       </c>
       <c r="I63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="3:13" x14ac:dyDescent="0.2">
       <c r="J64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K64" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="8:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="8:12" x14ac:dyDescent="0.2">
@@ -1819,134 +1828,134 @@
     </row>
     <row r="71" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J71" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L71" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K72" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L72" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J73" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L73" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J74" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L74" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J76" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K77" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K79" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K80" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="8:12" x14ac:dyDescent="0.2">
@@ -1954,7 +1963,7 @@
         <v>8</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="8:12" x14ac:dyDescent="0.2">
@@ -1978,7 +1987,7 @@
         <v>11</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="8:12" x14ac:dyDescent="0.2">
@@ -1993,39 +2002,39 @@
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
       <c r="J89" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K89" t="s">
+        <v>121</v>
+      </c>
+      <c r="L89" t="s">
         <v>123</v>
-      </c>
-      <c r="L89" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="90" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
       <c r="J90" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K90" t="s">
+        <v>122</v>
+      </c>
+      <c r="L90" t="s">
         <v>124</v>
-      </c>
-      <c r="L90" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="91" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
       <c r="J91" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K91" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L91" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="8:12" x14ac:dyDescent="0.2">
@@ -2034,7 +2043,7 @@
     </row>
     <row r="93" spans="8:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="J93" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>